<commit_message>
Importing is now fully tested
Also adds students to the student group
</commit_message>
<xml_diff>
--- a/test/support/import.xlsx
+++ b/test/support/import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/development/webCAT/test/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2E2601-D07B-5E49-A3D1-61D35F87AE4F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE38BB9-DEA8-5947-BAAD-F74A2941D092}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="6" xr2:uid="{53AC9FF3-DB18-3F40-8AF5-E780DB20391A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="7" xr2:uid="{53AC9FF3-DB18-3F40-8AF5-E780DB20391A}"/>
   </bookViews>
   <sheets>
     <sheet name="classrooms" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>id</t>
   </si>
@@ -82,21 +82,12 @@
     <t>semester_id</t>
   </si>
   <si>
-    <t>Test rotation from import</t>
-  </si>
-  <si>
-    <t>Test section from import</t>
-  </si>
-  <si>
     <t>section_id</t>
   </si>
   <si>
     <t>rotation_id</t>
   </si>
   <si>
-    <t>Test rotation group for import</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -136,12 +127,6 @@
     <t>Sub Category</t>
   </si>
   <si>
-    <t>Test sub-category from import</t>
-  </si>
-  <si>
-    <t>Test category for import</t>
-  </si>
-  <si>
     <t>content</t>
   </si>
   <si>
@@ -173,6 +158,24 @@
   </si>
   <si>
     <t>Test feedback</t>
+  </si>
+  <si>
+    <t>Test semester</t>
+  </si>
+  <si>
+    <t>Test section</t>
+  </si>
+  <si>
+    <t>Test rotation</t>
+  </si>
+  <si>
+    <t>Test rotation group</t>
+  </si>
+  <si>
+    <t>Test sub-category</t>
+  </si>
+  <si>
+    <t>Test category</t>
   </si>
 </sst>
 </file>
@@ -539,7 +542,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,10 +586,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE19661-95F9-DA4B-BA9E-8E4F35BA4D9B}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F1" sqref="F1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,7 +597,7 @@
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -610,8 +613,11 @@
       <c r="E1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -627,8 +633,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -643,6 +652,9 @@
       </c>
       <c r="E3">
         <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -655,7 +667,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -698,7 +710,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,7 +732,7 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -731,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1">
         <v>43470</v>
@@ -753,7 +765,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,7 +781,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -780,7 +792,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -796,7 +808,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -806,19 +818,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -826,19 +838,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -853,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D65138D-0C7A-B844-A051-2DEED4262819}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -877,7 +889,7 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -885,10 +897,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -899,10 +911,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -920,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C00CD22-880B-9D44-890C-223C220D90A2}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,13 +943,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -945,10 +957,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -959,10 +971,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -973,10 +985,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -992,7 +1004,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1005,10 +1017,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1016,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>1</v>

</xml_diff>